<commit_message>
Added another repo name in input file
</commit_message>
<xml_diff>
--- a/input_migration/File-Replacement1.xlsx
+++ b/input_migration/File-Replacement1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\production\input_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621DDDA3-A7BF-4D58-B458-504B65D569BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5499EEB-7C19-4767-B7C6-7DBA7603BF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Repository</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>seventhgithubrepo</t>
+  </si>
+  <si>
+    <t>production</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,6 +488,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Trying to replace the old Digital org
</commit_message>
<xml_diff>
--- a/input_migration/File-Replacement1.xlsx
+++ b/input_migration/File-Replacement1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\production\input_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5499EEB-7C19-4767-B7C6-7DBA7603BF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A367AF14-38E6-4164-AA0A-C11D6C213B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Repository</t>
   </si>
@@ -70,6 +70,33 @@
   </si>
   <si>
     <t>production</t>
+  </si>
+  <si>
+    <t>Exclude Strings</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\nx-affected-action</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\cf-tf-module-s3-website</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\cf-tf-module-ecs</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\testing123</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\JamesRepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\DeSilvaRepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\RanjanRepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital\Testing12345</t>
   </si>
 </sst>
 </file>
@@ -387,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,9 +425,10 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +438,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -421,8 +452,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,8 +466,11 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -443,8 +480,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -454,8 +494,11 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -465,8 +508,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -476,8 +522,11 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -487,8 +536,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -497,6 +549,9 @@
       </c>
       <c r="C9" t="s">
         <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>